<commit_message>
Vicks order XML and E2E Scenarios
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/Vicks/VicksTestData.xlsx
+++ b/src/test/resources/TestData/Vicks/VicksTestData.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cent_avayugundla\Documents\BVT\HoT-digital\src\test\resources\TestData\Vicks\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cent_avayugundla\Documents\git new code\HoT-digital\src\test\resources\TestData\Vicks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAA84FBA-2CEF-459D-8E44-9FA4222CA193}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{175F32E7-A10B-44D4-B288-08DADE609616}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="23280" windowHeight="12000" xr2:uid="{6632055E-F00D-4BCF-9FB6-5BE8B9EEFE1F}"/>
   </bookViews>
@@ -438,9 +438,6 @@
     <t>suvarchala</t>
   </si>
   <si>
-    <t>3Z9R773R25</t>
-  </si>
-  <si>
     <t>SalesMenu</t>
   </si>
   <si>
@@ -469,6 +466,9 @@
   </si>
   <si>
     <t>Humidifiers &amp; Vaporizers,Sinus Inhaler,Thermometers,Filters &amp; Accessories</t>
+  </si>
+  <si>
+    <t>3Z9R773R26</t>
   </si>
 </sst>
 </file>
@@ -940,8 +940,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4AD5157E-5E25-478E-8C85-BEF4818B37AA}">
   <dimension ref="A1:AO34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="S1" sqref="S1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1107,7 +1107,7 @@
         <v>134</v>
       </c>
       <c r="AO1" s="4" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="2" spans="1:41">
@@ -1165,7 +1165,7 @@
         <v>36</v>
       </c>
       <c r="F3" s="6" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="G3" s="5"/>
       <c r="H3" s="5"/>
@@ -1255,7 +1255,7 @@
         <v>36</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="G5" s="7"/>
       <c r="H5" s="7"/>
@@ -1723,13 +1723,13 @@
         <v>42</v>
       </c>
       <c r="S16" s="8">
-        <v>2025</v>
+        <v>2021</v>
       </c>
       <c r="T16" s="5" t="s">
         <v>43</v>
       </c>
       <c r="U16" s="8">
-        <v>369</v>
+        <v>365</v>
       </c>
       <c r="V16" s="5"/>
       <c r="W16" s="5"/>
@@ -1755,7 +1755,7 @@
         <v>33</v>
       </c>
       <c r="G17" s="21" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="H17" s="5"/>
       <c r="I17" s="5"/>
@@ -1895,7 +1895,7 @@
         <v>92</v>
       </c>
       <c r="G20" s="15" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="H20" s="15"/>
     </row>
@@ -1973,7 +1973,7 @@
         <v>36</v>
       </c>
       <c r="F28" s="6" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="G28" s="5"/>
       <c r="H28" s="5"/>
@@ -2004,7 +2004,7 @@
         <v>136</v>
       </c>
       <c r="C29" s="19" t="s">
-        <v>137</v>
+        <v>147</v>
       </c>
     </row>
     <row r="30" spans="1:41">
@@ -2057,26 +2057,26 @@
     </row>
     <row r="32" spans="1:41">
       <c r="A32" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="AO32" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="33" spans="1:41">
       <c r="A33" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="AO33" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="34" spans="1:41">
       <c r="A34" t="s">
+        <v>143</v>
+      </c>
+      <c r="G34" s="22" t="s">
         <v>144</v>
-      </c>
-      <c r="G34" s="22" t="s">
-        <v>145</v>
       </c>
     </row>
   </sheetData>

</xml_diff>